<commit_message>
- Weekely and bi-weekely practice contest.
</commit_message>
<xml_diff>
--- a/src/com/interview/excel/DS problem for interview.xlsx
+++ b/src/com/interview/excel/DS problem for interview.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="1276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="1337">
   <si>
     <t>Problem Name</t>
   </si>
@@ -3840,9 +3840,6 @@
     <t>MaxPerformanceOfTeam</t>
   </si>
   <si>
-    <t>Random HashMap Based/Array qut.</t>
-  </si>
-  <si>
     <t>BulbSwitcherIII</t>
   </si>
   <si>
@@ -3880,6 +3877,192 @@
   </si>
   <si>
     <t>GroupAnagrams</t>
+  </si>
+  <si>
+    <t>ProductOfLastKNums</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/product-of-the-last-k-numbers/</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.contest176</t>
+  </si>
+  <si>
+    <t>last K element retrival design using list..</t>
+  </si>
+  <si>
+    <t>MaxNumOfEvents</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-number-of-events-that-can-be-attended/</t>
+  </si>
+  <si>
+    <t>PQ to maintain timeline of events..</t>
+  </si>
+  <si>
+    <t>ConstructTargetArray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-target-array-with-multiple-sums/</t>
+  </si>
+  <si>
+    <t>Handling recursive problem using PQ.</t>
+  </si>
+  <si>
+    <t>ConstructPalindromeStrings</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-23/problems/construct-k-palindrome-strings/</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.biweekly.biweekely23</t>
+  </si>
+  <si>
+    <t>Conrtruct Palindrome Logic</t>
+  </si>
+  <si>
+    <t>ReducingDishes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reducing-dishes/</t>
+  </si>
+  <si>
+    <t>sorting + greedy pick</t>
+  </si>
+  <si>
+    <t>Greedy Based</t>
+  </si>
+  <si>
+    <t>CinemaSeatAllocation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/cinema-seat-allocation/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> com.interview.leetcode.contests.biweekly.biweekely22</t>
+  </si>
+  <si>
+    <t>Proper use of HashMap in place of Arrays.</t>
+  </si>
+  <si>
+    <t>IncreaseDecreaseString</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-21/problems/increasing-decreasing-string/</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.biweekly.biweekely21</t>
+  </si>
+  <si>
+    <t>Tricky string manipulation</t>
+  </si>
+  <si>
+    <t>LongestZigZagPaths</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-21/problems/longest-zigzag-path-in-a-binary-tree/</t>
+  </si>
+  <si>
+    <t>Tree with Traversing States.</t>
+  </si>
+  <si>
+    <t>CloneGraph</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/clone-graph/</t>
+  </si>
+  <si>
+    <t>Simple graph cloning.</t>
+  </si>
+  <si>
+    <t>SortByNumOfBits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-20/problems/sort-integers-by-the-number-of-1-bits/</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.biweekly.biweekely20</t>
+  </si>
+  <si>
+    <t>Count and sort by num of bits</t>
+  </si>
+  <si>
+    <t>ApplyDiscountNOrders</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/apply-discount-every-n-orders/</t>
+  </si>
+  <si>
+    <t>Easy Mapping using HashMap</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/apply-discount-every-n-orders/discuss/516982/Java-Straight-forward-Store-price-in-Hashmap</t>
+  </si>
+  <si>
+    <t>CountAllValidPickup</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-20/problems/count-all-valid-pickup-and-delivery-options/</t>
+  </si>
+  <si>
+    <t>Number of ways to Pick items : Permutations.</t>
+  </si>
+  <si>
+    <t>ShortestPathInGrid</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shortest-path-in-a-grid-with-obstacles-elimination/</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.bfs</t>
+  </si>
+  <si>
+    <t>BFS with K items delete..</t>
+  </si>
+  <si>
+    <t>JumpGameIV</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-19/problems/jump-game-iv/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> com.interview.codechef.ccdsap_2.leetcode.bfs</t>
+  </si>
+  <si>
+    <t>Jump in Array using BFS trick..</t>
+  </si>
+  <si>
+    <t>Random HashMap Based</t>
+  </si>
+  <si>
+    <t>RankTransformArray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-18/problems/rank-transform-of-an-array/</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.biweekly.biweekely18</t>
+  </si>
+  <si>
+    <t>Array Rank using Map</t>
+  </si>
+  <si>
+    <t>BreakAPalindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/break-a-palindrome/</t>
+  </si>
+  <si>
+    <t>Break Palindrome Lexicographically</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-the-matrix-diagonally/</t>
+  </si>
+  <si>
+    <t>Almost same as DiagonalTraverseII</t>
+  </si>
+  <si>
+    <t>SortMatrixDiagonally</t>
   </si>
 </sst>
 </file>
@@ -4370,15 +4553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" customWidth="1"/>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
     <col min="2" max="2" width="41.7265625" customWidth="1"/>
     <col min="3" max="3" width="66.54296875" customWidth="1"/>
     <col min="5" max="5" width="70.26953125" bestFit="1" customWidth="1"/>
@@ -4978,7 +5161,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>109</v>
@@ -5029,7 +5212,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>119</v>
@@ -5906,76 +6089,112 @@
         <v>957</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="9" t="s">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" s="17" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D110" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" s="17" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D111" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="17" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D112" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="9" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>964</v>
       </c>
-      <c r="B114" s="10" t="s">
+      <c r="B117" s="10" t="s">
         <v>965</v>
       </c>
-      <c r="C114" s="17" t="s">
+      <c r="C117" s="17" t="s">
         <v>966</v>
       </c>
-      <c r="D114" t="s">
-        <v>8</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="D117" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A115" s="17" t="s">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="17" t="s">
         <v>1086</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>1087</v>
       </c>
-      <c r="C115" s="17" t="s">
+      <c r="C118" s="17" t="s">
         <v>966</v>
       </c>
-      <c r="D115" t="s">
-        <v>8</v>
-      </c>
-      <c r="E115" t="s">
+      <c r="D118" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" t="s">
         <v>1088</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A116" s="17" t="s">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="17" t="s">
         <v>1111</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>1112</v>
       </c>
-      <c r="C116" s="17" t="s">
+      <c r="C119" s="17" t="s">
         <v>1113</v>
       </c>
-      <c r="D116" t="s">
-        <v>8</v>
-      </c>
-      <c r="E116" t="s">
+      <c r="D119" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="17"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="17"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A118" s="17"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="17"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A119" s="17"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="17"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="17"/>
@@ -5992,68 +6211,32 @@
       <c r="B122" s="3"/>
       <c r="C122" s="17"/>
     </row>
-    <row r="125" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="9" t="s">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" s="17"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="17"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" s="17"/>
+      <c r="B124" s="3"/>
+      <c r="C124" s="17"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" s="17"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="17"/>
+    </row>
+    <row r="128" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="9" t="s">
         <v>1016</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A126" s="17" t="s">
-        <v>629</v>
-      </c>
-      <c r="B126" s="20" t="s">
-        <v>1017</v>
-      </c>
-      <c r="C126" s="17" t="s">
-        <v>614</v>
-      </c>
-      <c r="D126" t="s">
-        <v>12</v>
-      </c>
-      <c r="E126" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A127" s="17" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>1020</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>892</v>
-      </c>
-      <c r="D127" t="s">
-        <v>12</v>
-      </c>
-      <c r="E127" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B128" s="10" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C128" s="17" t="s">
-        <v>614</v>
-      </c>
-      <c r="D128" t="s">
-        <v>12</v>
-      </c>
-      <c r="E128" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="17" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B129" s="13" t="s">
-        <v>1025</v>
+        <v>629</v>
+      </c>
+      <c r="B129" s="20" t="s">
+        <v>1017</v>
       </c>
       <c r="C129" s="17" t="s">
         <v>614</v>
@@ -6062,114 +6245,270 @@
         <v>12</v>
       </c>
       <c r="E129" t="s">
-        <v>337</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="17" t="s">
-        <v>627</v>
-      </c>
-      <c r="B130" s="10" t="s">
-        <v>628</v>
-      </c>
-      <c r="C130" s="17" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="D130" t="s">
+        <v>12</v>
+      </c>
+      <c r="E130" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C131" s="17" t="s">
         <v>614</v>
       </c>
-      <c r="D130" t="s">
-        <v>12</v>
-      </c>
-      <c r="E130" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A131" s="17" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>1083</v>
-      </c>
       <c r="D131" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E131" t="s">
-        <v>1084</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="17" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B132" s="13" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C132" s="17" t="s">
+        <v>614</v>
+      </c>
+      <c r="D132" t="s">
+        <v>12</v>
+      </c>
+      <c r="E132" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B133" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="C133" s="17" t="s">
+        <v>614</v>
+      </c>
+      <c r="D133" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" s="17" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C134" s="17" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D134" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="B135" s="3" t="s">
         <v>1103</v>
       </c>
-      <c r="C132" s="17" t="s">
+      <c r="C135" s="17" t="s">
         <v>1083</v>
       </c>
-      <c r="D132" t="s">
-        <v>8</v>
-      </c>
-      <c r="E132" t="s">
+      <c r="D135" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" t="s">
         <v>1104</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="9" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" s="17" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C136" s="17" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D136" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="9" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D142" t="s">
+        <v>12</v>
+      </c>
+      <c r="E142" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" s="17" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D143" t="s">
+        <v>12</v>
+      </c>
+      <c r="E143" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" s="17"/>
+      <c r="B144" s="3"/>
+      <c r="C144" s="4"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145" s="17"/>
+      <c r="B145" s="3"/>
+      <c r="C145" s="4"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" s="17"/>
+      <c r="B146" s="3"/>
+      <c r="C146" s="4"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" s="17" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C150" s="17" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D150" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151" s="17" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C151" s="17" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D151" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" s="17" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C152" s="17" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D152" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="9" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160" s="17" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D160" t="s">
+        <v>12</v>
+      </c>
+      <c r="E160" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" s="17" t="s">
         <v>1262</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A139" s="17" t="s">
-        <v>1115</v>
-      </c>
-      <c r="B139" s="10" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C139" s="17" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D139" t="s">
-        <v>8</v>
-      </c>
-      <c r="E139" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A140" s="17" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>1253</v>
-      </c>
-      <c r="D140" t="s">
-        <v>12</v>
-      </c>
-      <c r="E140" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A141" s="17" t="s">
+      <c r="B161" s="20" t="s">
         <v>1263</v>
       </c>
-      <c r="B141" s="20" t="s">
+      <c r="C161" s="17" t="s">
         <v>1264</v>
       </c>
-      <c r="C141" s="17" t="s">
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" t="s">
         <v>1265</v>
-      </c>
-      <c r="D141" t="s">
-        <v>8</v>
-      </c>
-      <c r="E141" t="s">
-        <v>1266</v>
       </c>
     </row>
   </sheetData>
@@ -6245,30 +6584,38 @@
     <hyperlink ref="B94" r:id="rId69"/>
     <hyperlink ref="B82" r:id="rId70"/>
     <hyperlink ref="B109" r:id="rId71"/>
-    <hyperlink ref="B127" r:id="rId72"/>
-    <hyperlink ref="B129" r:id="rId73"/>
-    <hyperlink ref="B131" r:id="rId74"/>
-    <hyperlink ref="B115" r:id="rId75"/>
-    <hyperlink ref="B132" r:id="rId76"/>
-    <hyperlink ref="B116" r:id="rId77"/>
+    <hyperlink ref="B130" r:id="rId72"/>
+    <hyperlink ref="B132" r:id="rId73"/>
+    <hyperlink ref="B134" r:id="rId74"/>
+    <hyperlink ref="B118" r:id="rId75"/>
+    <hyperlink ref="B135" r:id="rId76"/>
+    <hyperlink ref="B119" r:id="rId77"/>
     <hyperlink ref="B59" r:id="rId78"/>
     <hyperlink ref="C59" r:id="rId79"/>
     <hyperlink ref="B60" r:id="rId80"/>
     <hyperlink ref="B86" r:id="rId81"/>
     <hyperlink ref="B61" r:id="rId82"/>
-    <hyperlink ref="B140" r:id="rId83"/>
+    <hyperlink ref="B160" r:id="rId83"/>
+    <hyperlink ref="B136" r:id="rId84"/>
+    <hyperlink ref="B151" r:id="rId85"/>
+    <hyperlink ref="B111" r:id="rId86"/>
+    <hyperlink ref="B142" r:id="rId87"/>
+    <hyperlink ref="C142" r:id="rId88"/>
+    <hyperlink ref="B143" r:id="rId89"/>
+    <hyperlink ref="B112" r:id="rId90"/>
+    <hyperlink ref="B152" r:id="rId91"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId84"/>
+  <pageSetup orientation="portrait" r:id="rId92"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6323,21 +6670,39 @@
         <v>1099</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1310</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6542,19 +6907,36 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>1270</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>1271</v>
-      </c>
       <c r="C15" s="17" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="D15" t="s">
         <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>1272</v>
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="17" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1306</v>
       </c>
     </row>
   </sheetData>
@@ -6575,10 +6957,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6967,6 +7349,23 @@
       </c>
       <c r="E25" t="s">
         <v>1183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="17" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1278</v>
       </c>
     </row>
   </sheetData>
@@ -6988,9 +7387,10 @@
     <hyperlink ref="B19" r:id="rId15"/>
     <hyperlink ref="B21" r:id="rId16"/>
     <hyperlink ref="B24" r:id="rId17"/>
+    <hyperlink ref="B28" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -7219,7 +7619,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>1035</v>
@@ -9307,10 +9707,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9350,7 +9750,7 @@
       <c r="B3" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="17" t="s">
         <v>614</v>
       </c>
       <c r="D3" t="s">
@@ -9367,7 +9767,7 @@
       <c r="B4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="17" t="s">
         <v>619</v>
       </c>
       <c r="D4" t="s">
@@ -9384,7 +9784,7 @@
       <c r="B5" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>614</v>
       </c>
       <c r="D5" t="s">
@@ -9401,7 +9801,7 @@
       <c r="B6" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="17" t="s">
         <v>614</v>
       </c>
       <c r="D6" t="s">
@@ -9418,7 +9818,7 @@
       <c r="B7" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="17" t="s">
         <v>614</v>
       </c>
       <c r="D7" t="s">
@@ -9435,7 +9835,7 @@
       <c r="B8" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="17" t="s">
         <v>635</v>
       </c>
       <c r="D8" t="s">
@@ -9452,7 +9852,7 @@
       <c r="B9" s="3" t="s">
         <v>895</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="17" t="s">
         <v>892</v>
       </c>
       <c r="D9" t="s">
@@ -9469,7 +9869,7 @@
       <c r="B10" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>110</v>
       </c>
       <c r="D10" t="s">
@@ -9486,7 +9886,7 @@
       <c r="B11" s="3" t="s">
         <v>995</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="17" t="s">
         <v>996</v>
       </c>
       <c r="D11" t="s">
@@ -9503,7 +9903,7 @@
       <c r="B12" s="3" t="s">
         <v>1259</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="17" t="s">
         <v>1253</v>
       </c>
       <c r="D12" t="s">
@@ -9514,8 +9914,21 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
+      <c r="A13" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1281</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
@@ -9599,6 +10012,23 @@
       </c>
       <c r="E23" t="s">
         <v>632</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="17" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1284</v>
       </c>
     </row>
   </sheetData>
@@ -9618,9 +10048,11 @@
     <hyperlink ref="B9" r:id="rId13"/>
     <hyperlink ref="B11" r:id="rId14"/>
     <hyperlink ref="B12" r:id="rId15"/>
+    <hyperlink ref="B13" r:id="rId16"/>
+    <hyperlink ref="B28" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -10009,10 +10441,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10289,63 +10721,56 @@
         <v>664</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="17"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="17"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="17"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>986</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>985</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>987</v>
       </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
         <v>987</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="17" t="s">
-        <v>1089</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="17" t="s">
-        <v>1092</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" t="s">
-        <v>1094</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>1100</v>
+        <v>1089</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1101</v>
+        <v>1090</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>1083</v>
@@ -10354,15 +10779,15 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>1102</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>1118</v>
+        <v>1092</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1119</v>
+        <v>1093</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>1083</v>
@@ -10371,41 +10796,92 @@
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>1120</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>1213</v>
+        <v>1100</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>1215</v>
+        <v>1101</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>1083</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>1216</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="17" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="17" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>1267</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C41" s="17" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
         <v>1268</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>1265</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" t="s">
-        <v>1269</v>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="17" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1321</v>
       </c>
     </row>
   </sheetData>
@@ -10421,16 +10897,18 @@
     <hyperlink ref="B27" r:id="rId9"/>
     <hyperlink ref="B28" r:id="rId10"/>
     <hyperlink ref="B29" r:id="rId11"/>
-    <hyperlink ref="B33" r:id="rId12"/>
-    <hyperlink ref="B34" r:id="rId13"/>
-    <hyperlink ref="B35" r:id="rId14"/>
-    <hyperlink ref="B36" r:id="rId15"/>
-    <hyperlink ref="B37" r:id="rId16"/>
-    <hyperlink ref="B38" r:id="rId17"/>
-    <hyperlink ref="B39" r:id="rId18"/>
+    <hyperlink ref="B35" r:id="rId12"/>
+    <hyperlink ref="B36" r:id="rId13"/>
+    <hyperlink ref="B37" r:id="rId14"/>
+    <hyperlink ref="B38" r:id="rId15"/>
+    <hyperlink ref="B39" r:id="rId16"/>
+    <hyperlink ref="B40" r:id="rId17"/>
+    <hyperlink ref="B41" r:id="rId18"/>
+    <hyperlink ref="B42" r:id="rId19"/>
+    <hyperlink ref="B30" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -10438,8 +10916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11491,14 +11969,38 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="17"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="4"/>
+      <c r="A73" t="s">
+        <v>733</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="D73" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="17"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="4"/>
+      <c r="A74" s="17" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1303</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="17"/>
@@ -11586,23 +12088,6 @@
       </c>
       <c r="E84" t="s">
         <v>605</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>733</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>735</v>
-      </c>
-      <c r="D86" t="s">
-        <v>8</v>
-      </c>
-      <c r="E86" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -11751,8 +12236,8 @@
     <hyperlink ref="B68" r:id="rId52"/>
     <hyperlink ref="B69" r:id="rId53"/>
     <hyperlink ref="B70" r:id="rId54"/>
-    <hyperlink ref="B86" r:id="rId55"/>
-    <hyperlink ref="C86" r:id="rId56"/>
+    <hyperlink ref="B73" r:id="rId55"/>
+    <hyperlink ref="C73" r:id="rId56"/>
     <hyperlink ref="B41" r:id="rId57"/>
     <hyperlink ref="B29" r:id="rId58"/>
     <hyperlink ref="B95" r:id="rId59"/>
@@ -11763,9 +12248,10 @@
     <hyperlink ref="B72" r:id="rId64"/>
     <hyperlink ref="B42" r:id="rId65"/>
     <hyperlink ref="C42" r:id="rId66"/>
+    <hyperlink ref="B74" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId67"/>
+  <pageSetup orientation="portrait" r:id="rId68"/>
 </worksheet>
 </file>
 
@@ -11773,8 +12259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12460,6 +12946,23 @@
       </c>
       <c r="E62" t="s">
         <v>828</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="17" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D63" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1317</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -12754,9 +13257,10 @@
     <hyperlink ref="B88" r:id="rId38"/>
     <hyperlink ref="B101" r:id="rId39"/>
     <hyperlink ref="B102" r:id="rId40"/>
+    <hyperlink ref="B63" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId41"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
- Leetcode practice contest problems.
</commit_message>
<xml_diff>
--- a/src/com/interview/excel/DS problem for interview.xlsx
+++ b/src/com/interview/excel/DS problem for interview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="7250" tabRatio="677"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="7250" tabRatio="677" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Arr &amp; Str" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="1337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="1363">
   <si>
     <t>Problem Name</t>
   </si>
@@ -4063,6 +4063,84 @@
   </si>
   <si>
     <t>SortMatrixDiagonally</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/build-an-array-with-stack-operations/</t>
+  </si>
+  <si>
+    <t>BuildArray</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.contest188</t>
+  </si>
+  <si>
+    <t>Simple array implementation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-triplets-that-can-form-two-arrays-of-equal-xor/</t>
+  </si>
+  <si>
+    <t>MatrixSumBlock</t>
+  </si>
+  <si>
+    <t>Trick for Prefix sum on 2D array</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.biweekly.biweekely17</t>
+  </si>
+  <si>
+    <t>SumNodeOfEvenGrandParent</t>
+  </si>
+  <si>
+    <t>Simple Tree Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-17/problems/sum-of-nodes-with-even-valued-grandparent/</t>
+  </si>
+  <si>
+    <t>MinFlipsAOrB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> com.interview.leetcode.contests.contest171</t>
+  </si>
+  <si>
+    <t>Flip bits and counting</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-flips-to-make-a-or-b-equal-to-c/</t>
+  </si>
+  <si>
+    <t>DecryptString</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/weekly-contest-170/problems/decrypt-string-from-alphabet-to-integer-mapping/#</t>
+  </si>
+  <si>
+    <t>com.interview.leetcode.contests.contest170</t>
+  </si>
+  <si>
+    <t>Put a lot of Hardwork.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/weekly-contest-170/problems/xor-queries-of-a-subarray/</t>
+  </si>
+  <si>
+    <t>XORQueries</t>
+  </si>
+  <si>
+    <t>Solved by me.. :)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/biweekly-contest-17/problems/matrix-block-sum/</t>
+  </si>
+  <si>
+    <t>VideosWatchedByFriends</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/contest/weekly-contest-170/problems/get-watched-videos-by-your-friends/</t>
+  </si>
+  <si>
+    <t>Level Traversal using BFS, similar to Graph problem.</t>
   </si>
 </sst>
 </file>
@@ -4231,7 +4309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4272,6 +4350,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4553,10 +4632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6197,19 +6276,52 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A120" s="17"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="17"/>
+      <c r="A120" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D120" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A121" s="17"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="17"/>
+      <c r="A121" s="17" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B121" s="20" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D121" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" t="s">
+        <v>1343</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A122" s="17"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="17"/>
+      <c r="A122" s="17" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" t="s">
+        <v>1358</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="17"/>
@@ -6396,7 +6508,7 @@
       <c r="B143" s="3" t="s">
         <v>1328</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="C143" s="17" t="s">
         <v>1329</v>
       </c>
       <c r="D143" t="s">
@@ -6407,9 +6519,21 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" s="17"/>
-      <c r="B144" s="3"/>
-      <c r="C144" s="4"/>
+      <c r="A144" s="17" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C144" s="17" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D144" t="s">
+        <v>12</v>
+      </c>
+      <c r="E144" t="s">
+        <v>1355</v>
+      </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="17"/>
@@ -6484,7 +6608,7 @@
       <c r="B160" s="3" t="s">
         <v>1252</v>
       </c>
-      <c r="C160" s="4" t="s">
+      <c r="C160" s="17" t="s">
         <v>1253</v>
       </c>
       <c r="D160" t="s">
@@ -6496,18 +6620,70 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="17" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C161" s="17" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D161" t="s">
+        <v>12</v>
+      </c>
+      <c r="E161" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" s="17"/>
+      <c r="B162" s="3"/>
+      <c r="C162" s="4"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163" s="17"/>
+      <c r="B163" s="3"/>
+      <c r="C163" s="4"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164" s="17"/>
+      <c r="B164" s="3"/>
+      <c r="C164" s="4"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165" s="17"/>
+      <c r="B165" s="3"/>
+      <c r="C165" s="4"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" s="17"/>
+      <c r="B166" s="3"/>
+      <c r="C166" s="4"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167" s="17"/>
+      <c r="B167" s="3"/>
+      <c r="C167" s="4"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168" s="17"/>
+      <c r="B168" s="3"/>
+      <c r="C168" s="4"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" s="17" t="s">
         <v>1262</v>
       </c>
-      <c r="B161" s="20" t="s">
+      <c r="B169" s="20" t="s">
         <v>1263</v>
       </c>
-      <c r="C161" s="17" t="s">
+      <c r="C169" s="17" t="s">
         <v>1264</v>
       </c>
-      <c r="D161" t="s">
-        <v>8</v>
-      </c>
-      <c r="E161" t="s">
+      <c r="D169" t="s">
+        <v>8</v>
+      </c>
+      <c r="E169" t="s">
         <v>1265</v>
       </c>
     </row>
@@ -6604,24 +6780,28 @@
     <hyperlink ref="B143" r:id="rId89"/>
     <hyperlink ref="B112" r:id="rId90"/>
     <hyperlink ref="B152" r:id="rId91"/>
+    <hyperlink ref="B161" r:id="rId92"/>
+    <hyperlink ref="B120" r:id="rId93"/>
+    <hyperlink ref="B144" r:id="rId94" display="https://leetcode.com/contest/weekly-contest-170/problems/decrypt-string-from-alphabet-to-integer-mapping/"/>
+    <hyperlink ref="B122" r:id="rId95"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId92"/>
+  <pageSetup orientation="portrait" r:id="rId96"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="30.54296875" customWidth="1"/>
     <col min="5" max="5" width="36.26953125" customWidth="1"/>
   </cols>
@@ -6687,13 +6867,46 @@
         <v>1310</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1350</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -10441,10 +10654,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10882,6 +11095,23 @@
       </c>
       <c r="E42" t="s">
         <v>1321</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="17" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1362</v>
       </c>
     </row>
   </sheetData>
@@ -10916,8 +11146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81:C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10959,10 +11189,10 @@
       <c r="A5" t="s">
         <v>804</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>250</v>
       </c>
       <c r="D5" t="s">
@@ -10973,10 +11203,10 @@
       <c r="A6" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="20" t="s">
         <v>262</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="17" t="s">
         <v>250</v>
       </c>
       <c r="D6" t="s">
@@ -10987,15 +11217,21 @@
       <c r="A7" s="17" t="s">
         <v>805</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="17" t="s">
         <v>250</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -11004,7 +11240,7 @@
       <c r="B10" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D10" t="s">
@@ -11021,7 +11257,7 @@
       <c r="B11" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D11" t="s">
@@ -11038,7 +11274,7 @@
       <c r="B12" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D12" t="s">
@@ -11055,7 +11291,7 @@
       <c r="B13" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D13" t="s">
@@ -11072,7 +11308,7 @@
       <c r="B14" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D14" t="s">
@@ -11089,7 +11325,7 @@
       <c r="B15" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D15" t="s">
@@ -11106,7 +11342,7 @@
       <c r="B16" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D16" t="s">
@@ -11123,7 +11359,7 @@
       <c r="B17" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D17" t="s">
@@ -11140,7 +11376,7 @@
       <c r="B18" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D18" t="s">
@@ -11157,7 +11393,7 @@
       <c r="B19" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D19" t="s">
@@ -11174,7 +11410,7 @@
       <c r="B20" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D20" t="s">
@@ -11191,7 +11427,7 @@
       <c r="B21" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D21" t="s">
@@ -11208,7 +11444,7 @@
       <c r="B22" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D22" t="s">
@@ -11225,7 +11461,7 @@
       <c r="B23" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D23" t="s">
@@ -11242,7 +11478,7 @@
       <c r="B24" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D24" t="s">
@@ -11259,7 +11495,7 @@
       <c r="B25" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D25" t="s">
@@ -11276,7 +11512,7 @@
       <c r="B26" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D26" t="s">
@@ -11293,7 +11529,7 @@
       <c r="B27" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D27" t="s">
@@ -11310,7 +11546,7 @@
       <c r="B28" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D28" t="s">
@@ -11327,7 +11563,7 @@
       <c r="B29" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D29" t="s">
@@ -11353,7 +11589,7 @@
       <c r="B32" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D32" t="s">
@@ -11370,7 +11606,7 @@
       <c r="B33" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D33" t="s">
@@ -11387,7 +11623,7 @@
       <c r="B34" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D34" t="s">
@@ -11404,7 +11640,7 @@
       <c r="B35" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D35" t="s">
@@ -11421,7 +11657,7 @@
       <c r="B36" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D36" t="s">
@@ -11438,7 +11674,7 @@
       <c r="B37" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D37" t="s">
@@ -11455,7 +11691,7 @@
       <c r="B38" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D38" t="s">
@@ -11472,7 +11708,7 @@
       <c r="B39" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D39" t="s">
@@ -11489,7 +11725,7 @@
       <c r="B40" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D40" t="s">
@@ -11506,7 +11742,7 @@
       <c r="B41" s="3" t="s">
         <v>1003</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="17" t="s">
         <v>1004</v>
       </c>
       <c r="D41" t="s">
@@ -11545,7 +11781,7 @@
       <c r="B46" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D46" t="s">
@@ -11562,7 +11798,7 @@
       <c r="B47" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D47" t="s">
@@ -11579,7 +11815,7 @@
       <c r="B48" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D48" t="s">
@@ -11596,7 +11832,7 @@
       <c r="B49" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="17" t="s">
         <v>423</v>
       </c>
       <c r="D49" t="s">
@@ -11618,7 +11854,7 @@
       <c r="B52" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D52" t="s">
@@ -11635,7 +11871,7 @@
       <c r="B53" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D53" t="s">
@@ -11652,7 +11888,7 @@
       <c r="B54" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D54" t="s">
@@ -11669,7 +11905,7 @@
       <c r="B55" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D55" t="s">
@@ -11686,7 +11922,7 @@
       <c r="B56" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D56" t="s">
@@ -11703,7 +11939,7 @@
       <c r="B57" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D57" t="s">
@@ -11720,7 +11956,7 @@
       <c r="B58" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D58" t="s">
@@ -11737,7 +11973,7 @@
       <c r="B59" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D59" t="s">
@@ -11754,7 +11990,7 @@
       <c r="B60" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D60" t="s">
@@ -11771,7 +12007,7 @@
       <c r="B61" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D61" t="s">
@@ -11788,7 +12024,7 @@
       <c r="B62" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D62" t="s">
@@ -11805,7 +12041,7 @@
       <c r="B63" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D63" t="s">
@@ -11822,7 +12058,7 @@
       <c r="B64" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D64" t="s">
@@ -11839,7 +12075,7 @@
       <c r="B65" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D65" t="s">
@@ -11856,7 +12092,7 @@
       <c r="B66" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D66" t="s">
@@ -11873,7 +12109,7 @@
       <c r="B67" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D67" t="s">
@@ -11890,7 +12126,7 @@
       <c r="B68" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D68" t="s">
@@ -11907,7 +12143,7 @@
       <c r="B69" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D69" t="s">
@@ -11924,7 +12160,7 @@
       <c r="B70" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D70" t="s">
@@ -11941,7 +12177,7 @@
       <c r="B71" s="20" t="s">
         <v>1171</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="17" t="s">
         <v>1004</v>
       </c>
       <c r="D71" t="s">
@@ -11958,7 +12194,7 @@
       <c r="B72" s="3" t="s">
         <v>1203</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="17" t="s">
         <v>966</v>
       </c>
       <c r="D72" t="s">
@@ -11992,7 +12228,7 @@
       <c r="B74" s="3" t="s">
         <v>1302</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="17" t="s">
         <v>1299</v>
       </c>
       <c r="D74" t="s">
@@ -12003,9 +12239,21 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="17"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="4"/>
+      <c r="A75" s="17" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1346</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="17"/>
@@ -12029,7 +12277,7 @@
       <c r="B81" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D81" t="s">
@@ -12046,7 +12294,7 @@
       <c r="B82" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D82" t="s">
@@ -12063,7 +12311,7 @@
       <c r="B83" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="17" t="s">
         <v>591</v>
       </c>
       <c r="D83" t="s">
@@ -12249,9 +12497,10 @@
     <hyperlink ref="B42" r:id="rId65"/>
     <hyperlink ref="C42" r:id="rId66"/>
     <hyperlink ref="B74" r:id="rId67"/>
+    <hyperlink ref="B75" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId68"/>
+  <pageSetup orientation="portrait" r:id="rId69"/>
 </worksheet>
 </file>
 
@@ -12259,8 +12508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>